<commit_message>
Merge branches 'main' and 'main' of https://github.com/ecahyono/Automationpython
</commit_message>
<xml_diff>
--- a/SDP/Filexel/FakerGiatja.xlsx
+++ b/SDP/Filexel/FakerGiatja.xlsx
@@ -429,49 +429,49 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>jenisKegiatan2</t>
+          <t>jenisKegiatan1</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>Fugit.</t>
+          <t>Ipsa.</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>skala0</t>
+          <t>skala1</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>12/05/2023</t>
+          <t>16/05/2023</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>21/05/2023</t>
+          <t>24/05/2023</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>area2</t>
+          <t>area1</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>Gg. Jakarta No. 1
-Sungai Penuh, SU 60714</t>
+          <t>Jalan Rungkut Industri No. 90
+Kota Administrasi Jakarta Utara, Kalimantan Barat 01801</t>
         </is>
       </c>
       <c r="I1" t="n">
-        <v>375</v>
+        <v>345</v>
       </c>
       <c r="J1" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>sarana1</t>
+          <t>sarana0</t>
         </is>
       </c>
       <c r="L1" t="inlineStr">
@@ -486,50 +486,50 @@
       </c>
       <c r="N1" t="inlineStr">
         <is>
-          <t>Dolorum eaque sit nisi. Quo sequi libero maiores.</t>
+          <t>Voluptas occaecati eaque eum quae quo iusto. Eligendi quo sunt.</t>
         </is>
       </c>
       <c r="O1" t="n">
+        <v>1</v>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>.el-table__row:nth-child(7) .el-checkbox__inner</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>.el-table__row:nth-child(1) .el-checkbox__inner</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>.el-table__row:nth-child(6) .el-checkbox__inner</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>jenis1</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>Fuga.</t>
+        </is>
+      </c>
+      <c r="U1" t="n">
+        <v>1</v>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>satuan5</t>
+        </is>
+      </c>
+      <c r="W1" t="n">
+        <v>341121</v>
+      </c>
+      <c r="X1" t="n">
         <v>2</v>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>.el-table__row:nth-child(8) .el-checkbox__inner</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>.el-table__row:nth-child(1) .el-checkbox__inner</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>.el-table__row:nth-child(8) .el-checkbox__inner</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>#jenis1 &gt; span</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>Eum.</t>
-        </is>
-      </c>
-      <c r="U1" t="n">
-        <v>3</v>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>satuan5</t>
-        </is>
-      </c>
-      <c r="W1" t="n">
-        <v>605148</v>
-      </c>
-      <c r="X1" t="n">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>